<commit_message>
Atualização automática - 01/03/2026 23:06
</commit_message>
<xml_diff>
--- a/dados/16 a 22-02/ENTREGAS_DIA.xlsx
+++ b/dados/16 a 22-02/ENTREGAS_DIA.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29628"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29725"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Python\Dashboard_Sauipe\dados\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/b754a023a117f00d/Documentos/python/Projetos/Dashboard_Sauipe - Copia/dados/16 a 22-02/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B4BECFE6-6D35-4409-8DEE-35944F46F5D2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="21" documentId="13_ncr:1_{B4BECFE6-6D35-4409-8DEE-35944F46F5D2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B855B092-7F40-4B34-9D2F-045F2E70B453}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Totais" sheetId="1" r:id="rId1"/>
@@ -241,16 +241,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -279,6 +276,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -569,7 +570,7 @@
   <dimension ref="A1:B24"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="B25" sqref="B25"/>
     </sheetView>
   </sheetViews>
@@ -591,7 +592,7 @@
       <c r="A2" s="2">
         <v>46054</v>
       </c>
-      <c r="B2" s="3">
+      <c r="B2">
         <v>437</v>
       </c>
     </row>
@@ -599,7 +600,7 @@
       <c r="A3" s="2">
         <v>46055</v>
       </c>
-      <c r="B3" s="3">
+      <c r="B3">
         <v>340</v>
       </c>
     </row>
@@ -607,7 +608,7 @@
       <c r="A4" s="2">
         <v>46056</v>
       </c>
-      <c r="B4" s="3">
+      <c r="B4">
         <v>349</v>
       </c>
     </row>
@@ -615,7 +616,7 @@
       <c r="A5" s="2">
         <v>46057</v>
       </c>
-      <c r="B5" s="3">
+      <c r="B5">
         <v>381</v>
       </c>
     </row>
@@ -623,7 +624,7 @@
       <c r="A6" s="2">
         <v>46058</v>
       </c>
-      <c r="B6" s="3">
+      <c r="B6">
         <v>344</v>
       </c>
     </row>
@@ -631,7 +632,7 @@
       <c r="A7" s="2">
         <v>46059</v>
       </c>
-      <c r="B7" s="3">
+      <c r="B7">
         <v>300</v>
       </c>
     </row>
@@ -639,7 +640,7 @@
       <c r="A8" s="2">
         <v>46060</v>
       </c>
-      <c r="B8" s="3">
+      <c r="B8">
         <v>264</v>
       </c>
     </row>
@@ -647,7 +648,7 @@
       <c r="A9" s="2">
         <v>46061</v>
       </c>
-      <c r="B9" s="3">
+      <c r="B9">
         <v>393</v>
       </c>
     </row>
@@ -655,7 +656,7 @@
       <c r="A10" s="2">
         <v>46062</v>
       </c>
-      <c r="B10" s="3">
+      <c r="B10">
         <v>310</v>
       </c>
     </row>
@@ -663,7 +664,7 @@
       <c r="A11" s="2">
         <v>46063</v>
       </c>
-      <c r="B11" s="3">
+      <c r="B11">
         <v>336</v>
       </c>
     </row>
@@ -671,7 +672,7 @@
       <c r="A12" s="2">
         <v>46064</v>
       </c>
-      <c r="B12" s="3">
+      <c r="B12">
         <v>320</v>
       </c>
     </row>
@@ -679,7 +680,7 @@
       <c r="A13" s="2">
         <v>46065</v>
       </c>
-      <c r="B13" s="3">
+      <c r="B13">
         <v>299</v>
       </c>
     </row>
@@ -687,7 +688,7 @@
       <c r="A14" s="2">
         <v>46066</v>
       </c>
-      <c r="B14" s="3">
+      <c r="B14">
         <v>285</v>
       </c>
     </row>
@@ -695,7 +696,7 @@
       <c r="A15" s="2">
         <v>46067</v>
       </c>
-      <c r="B15" s="3">
+      <c r="B15">
         <v>307</v>
       </c>
     </row>
@@ -764,10 +765,10 @@
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A24" s="4" t="s">
+      <c r="A24" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="B24" s="5">
+      <c r="B24" s="4">
         <f>SUM(B2:B23)</f>
         <v>7327</v>
       </c>
@@ -804,442 +805,442 @@
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A2" s="6" t="s">
+      <c r="A2" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="B2" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="C2" s="7">
+      <c r="B2" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C2" s="6">
         <v>33</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A3" s="6" t="s">
+      <c r="A3" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="B3" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="C3" s="7">
+      <c r="B3" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C3" s="6">
         <v>66</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A4" s="6" t="s">
+      <c r="A4" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="B4" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="C4" s="7">
+      <c r="B4" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C4" s="6">
         <v>1</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A5" s="6" t="s">
+      <c r="A5" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="B5" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="C5" s="7">
+      <c r="B5" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C5" s="6">
         <v>245</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A6" s="6" t="s">
+      <c r="A6" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="B6" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="C6" s="7">
+      <c r="B6" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C6" s="6">
         <v>10</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A7" s="6" t="s">
+      <c r="A7" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="B7" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="C7" s="7">
+      <c r="B7" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C7" s="6">
         <v>210</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A8" s="6" t="s">
+      <c r="A8" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="B8" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="C8" s="7">
+      <c r="B8" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C8" s="6">
         <v>191</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A9" s="6" t="s">
+      <c r="A9" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="B9" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="C9" s="7">
+      <c r="B9" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C9" s="6">
         <v>43</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A10" s="6" t="s">
+      <c r="A10" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="B10" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="C10" s="7">
+      <c r="B10" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C10" s="6">
         <v>17</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A11" s="6" t="s">
+      <c r="A11" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="B11" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="C11" s="7">
+      <c r="B11" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C11" s="6">
         <v>1852</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A12" s="6" t="s">
+      <c r="A12" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="B12" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="C12" s="7">
+      <c r="B12" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C12" s="6">
         <v>170</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A13" s="6" t="s">
+      <c r="A13" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="B13" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="C13" s="7">
+      <c r="B13" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C13" s="6">
         <v>1101</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A14" s="6" t="s">
+      <c r="A14" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="B14" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="C14" s="7">
+      <c r="B14" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C14" s="6">
         <v>139</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A15" s="6" t="s">
+      <c r="A15" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="B15" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="C15" s="7">
+      <c r="B15" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C15" s="6">
         <v>11</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A16" s="6" t="s">
+      <c r="A16" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="B16" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="C16" s="7">
+      <c r="B16" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C16" s="6">
         <v>14</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A17" s="6" t="s">
+      <c r="A17" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="B17" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="C17" s="7">
+      <c r="B17" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C17" s="6">
         <v>569</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A18" s="6" t="s">
+      <c r="A18" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="B18" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="C18" s="7">
+      <c r="B18" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C18" s="6">
         <v>64</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A19" s="6" t="s">
+      <c r="A19" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="B19" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="C19" s="7">
+      <c r="B19" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C19" s="6">
         <v>17</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A20" s="6" t="s">
+      <c r="A20" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="B20" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="C20" s="7">
+      <c r="B20" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C20" s="6">
         <v>1196</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A21" s="6" t="s">
+      <c r="A21" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="B21" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="C21" s="7">
+      <c r="B21" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C21" s="6">
         <v>59</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A22" s="6" t="s">
+      <c r="A22" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="B22" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="C22" s="7">
+      <c r="B22" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C22" s="6">
         <v>26</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A23" s="6" t="s">
+      <c r="A23" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="B23" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="C23" s="7">
+      <c r="B23" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C23" s="6">
         <v>12</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A24" s="6" t="s">
+      <c r="A24" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="B24" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="C24" s="7">
+      <c r="B24" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C24" s="6">
         <v>23</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A25" s="6" t="s">
+      <c r="A25" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="B25" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="C25" s="7">
+      <c r="B25" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C25" s="6">
         <v>2531</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A26" s="6" t="s">
+      <c r="A26" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="B26" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="C26" s="7">
+      <c r="B26" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C26" s="6">
         <v>376</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A27" s="6" t="s">
+      <c r="A27" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="B27" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="C27" s="7">
+      <c r="B27" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C27" s="6">
         <v>10</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A28" s="6" t="s">
+      <c r="A28" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="B28" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="C28" s="7">
+      <c r="B28" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C28" s="6">
         <v>9</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A29" s="6" t="s">
+      <c r="A29" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="B29" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="C29" s="7">
+      <c r="B29" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C29" s="6">
         <v>11</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A30" s="6" t="s">
+      <c r="A30" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="B30" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="C30" s="7">
+      <c r="B30" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C30" s="6">
         <v>86</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A31" s="6" t="s">
+      <c r="A31" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="B31" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="C31" s="7">
+      <c r="B31" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C31" s="6">
         <v>23</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A32" s="6" t="s">
+      <c r="A32" s="5" t="s">
         <v>37</v>
       </c>
-      <c r="B32" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="C32" s="7">
+      <c r="B32" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C32" s="6">
         <v>62</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A33" s="6" t="s">
+      <c r="A33" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="B33" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="C33" s="7">
+      <c r="B33" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C33" s="6">
         <v>94</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A34" s="6" t="s">
+      <c r="A34" s="5" t="s">
         <v>39</v>
       </c>
-      <c r="B34" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="C34" s="7">
+      <c r="B34" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C34" s="6">
         <v>41</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A35" s="6" t="s">
+      <c r="A35" s="5" t="s">
         <v>40</v>
       </c>
-      <c r="B35" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="C35" s="7">
+      <c r="B35" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C35" s="6">
         <v>65</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A36" s="6" t="s">
+      <c r="A36" s="5" t="s">
         <v>41</v>
       </c>
-      <c r="B36" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="C36" s="7">
+      <c r="B36" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C36" s="6">
         <v>20</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A37" s="6" t="s">
+      <c r="A37" s="5" t="s">
         <v>42</v>
       </c>
-      <c r="B37" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="C37" s="7">
+      <c r="B37" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C37" s="6">
         <v>133</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A38" s="6" t="s">
+      <c r="A38" s="5" t="s">
         <v>43</v>
       </c>
-      <c r="B38" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="C38" s="7">
+      <c r="B38" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C38" s="6">
         <v>10</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A39" s="6" t="s">
+      <c r="A39" s="5" t="s">
         <v>44</v>
       </c>
-      <c r="B39" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="C39" s="7">
+      <c r="B39" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C39" s="6">
         <v>919</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A40" s="6" t="s">
+      <c r="A40" s="5" t="s">
         <v>45</v>
       </c>
-      <c r="B40" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="C40" s="7">
+      <c r="B40" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C40" s="6">
         <v>31</v>
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A41" s="6" t="s">
+      <c r="A41" s="5" t="s">
         <v>46</v>
       </c>
-      <c r="B41" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="C41" s="7">
+      <c r="B41" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C41" s="6">
         <v>19</v>
       </c>
     </row>

</xml_diff>